<commit_message>
Crop rate outliers detection included.
</commit_message>
<xml_diff>
--- a/loop/impact scripts/Market Count Wise Impact.xlsx
+++ b/loop/impact scripts/Market Count Wise Impact.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19140" windowHeight="7090"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19140" windowHeight="7090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Market Count Wise Impact" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Market Count</t>
   </si>
@@ -35,6 +37,9 @@
   </si>
   <si>
     <t>Per Kg Delta</t>
+  </si>
+  <si>
+    <t>Visits %</t>
   </si>
 </sst>
 </file>
@@ -519,11 +524,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -605,6 +611,632 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Delta %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.16923398563399999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.0313223903</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.428578335200001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.364447106899998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.9712659797</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.435302330200003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.055246458500001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.891185168000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.778069318099995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.272547683599996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>74.226977810400001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="243401472"/>
+        <c:axId val="243403392"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Per Kg Delta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.6780646857400001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.04788883252</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6866403428500001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6699164193299998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.49374222447</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.64388483289</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6392885826799999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.2793618254999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2839244445400002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.7290347763399998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.61824493695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="243419776"/>
+        <c:axId val="243417856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="243401472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Markets with Available Rates</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="243403392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="243403392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Difference</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>in Amount</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="243401472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="243417856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Difference</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Per Kg</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="243419776"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="243419776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="243417856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1237</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="243432064"/>
+        <c:axId val="243442432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="243432064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> markets with available rates</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="243442432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="243442432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> market visits</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="243432064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>44449</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>555365</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171434</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="1104900"/>
+          <a:ext cx="7260965" cy="2749534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -896,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1329,4 +1961,375 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3197</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B2*100/B$13</f>
+        <v>50.593448330432032</v>
+      </c>
+      <c r="D2" s="1">
+        <v>50992093.112199999</v>
+      </c>
+      <c r="E2" s="1">
+        <v>50905942.956</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5133899.5999999996</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.16923398563399999</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.6780646857400001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1237</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C12" si="0">B3*100/B$13</f>
+        <v>19.575882259851241</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19827400.603100002</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17857483.975000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1879890.85</v>
+      </c>
+      <c r="G3" s="2">
+        <v>11.0313223903</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.04788883252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>701</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>11.093527456876089</v>
+      </c>
+      <c r="D4" s="1">
+        <v>11799421.4636</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10134471.8215</v>
+      </c>
+      <c r="F4" s="1">
+        <v>987139.7</v>
+      </c>
+      <c r="G4" s="2">
+        <v>16.428578335200001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.6866403428500001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>469</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4220604526032599</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8104913.9257100001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6465081.6979999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>614188.6</v>
+      </c>
+      <c r="G5" s="2">
+        <v>25.364447106899998</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.6699164193299998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>223</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5290394049691405</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3704454.5795900002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2785906.077</v>
+      </c>
+      <c r="F6" s="1">
+        <v>262912.5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>32.9712659797</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3.49374222447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>164</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5953473650894128</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2140015.7555900002</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1580101.878</v>
+      </c>
+      <c r="F7" s="1">
+        <v>153658.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>35.435302330200003</v>
+      </c>
+      <c r="H7" s="2">
+        <v>3.64388483289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>110</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7407817692672891</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1676109.3762399999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1139782.1000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <v>115605.5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>47.055246458500001</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4.6392885826799999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>104</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6458300363981642</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2091435.62583</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1137322.392</v>
+      </c>
+      <c r="F9" s="1">
+        <v>131071</v>
+      </c>
+      <c r="G9" s="2">
+        <v>83.891185168000007</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7.2793618254999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>70</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1077702168064567</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1764059.76829</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1020997.5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>102014</v>
+      </c>
+      <c r="G10" s="2">
+        <v>72.778069318099995</v>
+      </c>
+      <c r="H10" s="2">
+        <v>7.2839244445400002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4747586643456243</v>
+      </c>
+      <c r="D11" s="1">
+        <v>614561.05812299997</v>
+      </c>
+      <c r="E11" s="1">
+        <v>337166</v>
+      </c>
+      <c r="F11" s="1">
+        <v>35890</v>
+      </c>
+      <c r="G11" s="2">
+        <v>82.272547683599996</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7.7290347763399998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22155404336129134</v>
+      </c>
+      <c r="D12" s="1">
+        <v>216457.85496200001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>124239</v>
+      </c>
+      <c r="F12" s="1">
+        <v>12105</v>
+      </c>
+      <c r="G12" s="2">
+        <v>74.226977810400001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>7.61824493695</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <f>SUM(B2:B12)</f>
+        <v>6319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
impact evalution code with outliers integration with pandas
</commit_message>
<xml_diff>
--- a/loop/impact scripts/Market Count Wise Impact.xlsx
+++ b/loop/impact scripts/Market Count Wise Impact.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -702,8 +703,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243401472"/>
-        <c:axId val="243403392"/>
+        <c:axId val="126636800"/>
+        <c:axId val="126638720"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -780,11 +781,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243419776"/>
-        <c:axId val="243417856"/>
+        <c:axId val="126642816"/>
+        <c:axId val="126640896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243401472"/>
+        <c:axId val="126636800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -817,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243403392"/>
+        <c:crossAx val="126638720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -825,7 +826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243403392"/>
+        <c:axId val="126638720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,12 +865,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243401472"/>
+        <c:crossAx val="126636800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="243417856"/>
+        <c:axId val="126640896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,12 +909,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243419776"/>
+        <c:crossAx val="126642816"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="243419776"/>
+        <c:axId val="126642816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -922,7 +923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243417856"/>
+        <c:crossAx val="126640896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1034,11 +1035,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243432064"/>
-        <c:axId val="243442432"/>
+        <c:axId val="126683776"/>
+        <c:axId val="126690048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243432064"/>
+        <c:axId val="126683776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1072,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243442432"/>
+        <c:crossAx val="126690048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1079,7 +1080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243442432"/>
+        <c:axId val="126690048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1115,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243432064"/>
+        <c:crossAx val="126683776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>